<commit_message>
Make resistor networks more obvious.
</commit_message>
<xml_diff>
--- a/Modules/AxB/AxB_BOM.xlsx
+++ b/Modules/AxB/AxB_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\AxB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F14000D-C260-43E5-9E94-DDDA865B706E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ECE229-CFD9-4B06-8971-0BD2DF0F520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,9 +293,6 @@
     <t>R-Array-SIP8</t>
   </si>
   <si>
-    <t>Resistor Network THT, 4 Isolated Resistors</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/hr/en/details/dr100k-4_8/resistor-networks/royal-ohm/rnlb08g0104b0e/</t>
   </si>
   <si>
@@ -476,6 +473,21 @@
         <scheme val="minor"/>
       </rPr>
       <t>, R10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Resistor Network THT,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4 Isolated Resistors</t>
     </r>
   </si>
 </sst>
@@ -1377,7 +1389,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1434,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -1482,7 +1494,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -1502,16 +1514,16 @@
         <v>85</v>
       </c>
       <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="P6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1525,16 +1537,16 @@
         <v>85</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1542,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -1554,7 +1566,7 @@
         <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1568,7 +1580,7 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1648,7 +1660,7 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
@@ -1668,7 +1680,7 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
         <v>31</v>
@@ -1682,19 +1694,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
         <v>98</v>
       </c>
-      <c r="C15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1702,13 +1714,13 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
         <v>101</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E16" t="s">
         <v>78</v>
@@ -1728,7 +1740,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1742,19 +1754,19 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
         <v>111</v>
       </c>
-      <c r="C18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1768,7 +1780,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -1782,13 +1794,13 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
@@ -1808,7 +1820,7 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
@@ -1822,13 +1834,13 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -1848,7 +1860,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
@@ -1970,7 +1982,7 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E32" t="s">
         <v>62</v>
@@ -2003,12 +2015,12 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update BOMs with newer links and names.
</commit_message>
<xml_diff>
--- a/Modules/AxB/AxB_BOM.xlsx
+++ b/Modules/AxB/AxB_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\AxB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ECE229-CFD9-4B06-8971-0BD2DF0F520D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A35379E-3DC7-4EBA-821E-1C1F3F8307C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="122">
   <si>
     <t>Qty</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Potentiometer Nut</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/alpha-nuts-washers/</t>
   </si>
   <si>
     <t>Black D-Shaft Line</t>
@@ -489,6 +486,12 @@
       </rPr>
       <t xml:space="preserve"> 4 Isolated Resistors</t>
     </r>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/black-nuts-washers/</t>
+  </si>
+  <si>
+    <t>Thonkiconn</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1392,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1437,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -1448,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1468,13 +1471,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -1494,7 +1497,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -1508,22 +1511,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="P6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1534,19 +1537,19 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1554,7 +1557,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -1566,7 +1569,7 @@
         <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1580,7 +1583,7 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1660,7 +1663,7 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
@@ -1680,7 +1683,7 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
         <v>31</v>
@@ -1694,19 +1697,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
         <v>97</v>
       </c>
-      <c r="C15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1714,16 +1717,16 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
         <v>100</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>46</v>
@@ -1740,7 +1743,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1754,19 +1757,19 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" t="s">
         <v>110</v>
       </c>
-      <c r="C18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1774,13 +1777,13 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -1794,19 +1797,19 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,13 +1823,13 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,19 +1837,19 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,13 +1863,13 @@
         <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1886,7 +1889,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1894,16 +1897,16 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
         <v>65</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>66</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1911,16 +1914,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>71</v>
       </c>
-      <c r="E27" t="s">
-        <v>72</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,16 +1931,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1951,7 +1954,7 @@
         <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>56</v>
@@ -1968,7 +1971,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>58</v>
@@ -1982,13 +1985,13 @@
         <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E32" t="s">
         <v>62</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1996,7 +1999,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
         <v>60</v>
@@ -2015,12 +2018,12 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2040,23 +2043,23 @@
     <hyperlink ref="F30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="F31" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="F22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F20" r:id="rId17" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
-    <hyperlink ref="F24" r:id="rId18" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
-    <hyperlink ref="P6" r:id="rId19" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
-    <hyperlink ref="P7" r:id="rId20" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
-    <hyperlink ref="F7" r:id="rId21" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
-    <hyperlink ref="F6" r:id="rId22" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
-    <hyperlink ref="F8" r:id="rId23" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
-    <hyperlink ref="F15" r:id="rId24" xr:uid="{850880ED-5B0D-4785-BD00-D263FDB1367B}"/>
-    <hyperlink ref="F16" r:id="rId25" xr:uid="{53562666-7339-4495-85C8-BCFF4A8BDBAF}"/>
-    <hyperlink ref="F21" r:id="rId26" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
-    <hyperlink ref="F23" r:id="rId27" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
-    <hyperlink ref="F18" r:id="rId28" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
-    <hyperlink ref="F2" r:id="rId29" xr:uid="{9E0ED9E0-C3A3-4348-BB6F-5C429B9E61E7}"/>
-    <hyperlink ref="F5" r:id="rId30" xr:uid="{AC848EF4-7FAB-4E48-AF09-F798B5BC950A}"/>
-    <hyperlink ref="F3" r:id="rId31" xr:uid="{238CA172-A99C-46CD-9FBB-BE7CBE8D9023}"/>
-    <hyperlink ref="F4" r:id="rId32" xr:uid="{7C381042-415D-491B-ACA4-70B1B604E6FF}"/>
+    <hyperlink ref="F20" r:id="rId16" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
+    <hyperlink ref="F24" r:id="rId17" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
+    <hyperlink ref="P6" r:id="rId18" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
+    <hyperlink ref="P7" r:id="rId19" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
+    <hyperlink ref="F7" r:id="rId20" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
+    <hyperlink ref="F6" r:id="rId21" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
+    <hyperlink ref="F8" r:id="rId22" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
+    <hyperlink ref="F15" r:id="rId23" xr:uid="{850880ED-5B0D-4785-BD00-D263FDB1367B}"/>
+    <hyperlink ref="F16" r:id="rId24" xr:uid="{53562666-7339-4495-85C8-BCFF4A8BDBAF}"/>
+    <hyperlink ref="F21" r:id="rId25" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
+    <hyperlink ref="F23" r:id="rId26" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
+    <hyperlink ref="F18" r:id="rId27" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
+    <hyperlink ref="F2" r:id="rId28" xr:uid="{9E0ED9E0-C3A3-4348-BB6F-5C429B9E61E7}"/>
+    <hyperlink ref="F5" r:id="rId29" xr:uid="{AC848EF4-7FAB-4E48-AF09-F798B5BC950A}"/>
+    <hyperlink ref="F3" r:id="rId30" xr:uid="{238CA172-A99C-46CD-9FBB-BE7CBE8D9023}"/>
+    <hyperlink ref="F4" r:id="rId31" xr:uid="{7C381042-415D-491B-ACA4-70B1B604E6FF}"/>
+    <hyperlink ref="F32" r:id="rId32" xr:uid="{5285EE03-FF15-4800-B4FB-C302200D43C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>

</xml_diff>

<commit_message>
Label BOM items better.
</commit_message>
<xml_diff>
--- a/Modules/AxB/AxB_BOM.xlsx
+++ b/Modules/AxB/AxB_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\AxB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A35379E-3DC7-4EBA-821E-1C1F3F8307C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75F306A-8ABC-4EB6-9A89-45ACA2CF04F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,28 +101,13 @@
     <t>L-937EGW</t>
   </si>
   <si>
-    <t>R-W4</t>
-  </si>
-  <si>
     <t>Resistor THT</t>
   </si>
   <si>
-    <t>C-5mm</t>
-  </si>
-  <si>
-    <t>E2.5-6.3</t>
-  </si>
-  <si>
     <t>DO-41</t>
   </si>
   <si>
     <t>DO-35</t>
-  </si>
-  <si>
-    <t>Capacitor Polarized THT</t>
-  </si>
-  <si>
-    <t>Capacitor Ceramic THT</t>
   </si>
   <si>
     <t>DIP-14</t>
@@ -493,12 +478,27 @@
   <si>
     <t>Thonkiconn</t>
   </si>
+  <si>
+    <t>R-1/4W</t>
+  </si>
+  <si>
+    <t>Electrolytic Capacitor THT</t>
+  </si>
+  <si>
+    <t>E-P2.5mm 6.3x11.5mm</t>
+  </si>
+  <si>
+    <t>C-P5mm</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor THT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,13 +632,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1034,15 +1027,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1392,7 +1384,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E8" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,25 +1398,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1434,16 +1426,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>39</v>
+      <c r="F2" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1451,19 +1443,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>39</v>
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1471,19 +1463,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>39</v>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1494,16 +1486,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
+      <c r="F5" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1511,22 +1503,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1537,19 +1529,19 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>86</v>
+        <v>114</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1557,19 +1549,19 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>91</v>
+        <v>121</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1579,17 +1571,17 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
+      <c r="C9" t="s">
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>40</v>
+        <v>121</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1600,16 +1592,16 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>41</v>
+        <v>118</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1620,16 +1612,16 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1640,16 +1632,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1657,19 +1649,19 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>44</v>
+        <v>29</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -1680,16 +1672,16 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1697,19 +1689,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1717,19 +1709,19 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>46</v>
+        <v>72</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,14 +1734,14 @@
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>102</v>
+      <c r="D17" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>47</v>
+      <c r="F17" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,19 +1749,19 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,19 +1769,19 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>103</v>
+        <v>43</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,19 +1789,19 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>79</v>
+      <c r="F20" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,19 +1809,19 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>79</v>
+      <c r="F21" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1837,19 +1829,19 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>107</v>
+        <v>46</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>78</v>
+      <c r="F22" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,19 +1849,19 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>108</v>
+        <v>46</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>78</v>
+      <c r="F23" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1877,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -1888,8 +1880,8 @@
       <c r="E24" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>80</v>
+      <c r="F24" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,16 +1889,16 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,16 +1906,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1931,16 +1923,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1948,16 +1940,16 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>56</v>
+        <v>71</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,16 +1957,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>58</v>
+        <v>71</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1982,16 +1974,16 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>120</v>
+        <v>57</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1999,31 +1991,31 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>37</v>
+      <c r="B35" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>115</v>
+      <c r="B37" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>114</v>
+      <c r="B38" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleanup all BOMs and update with new URLs.
</commit_message>
<xml_diff>
--- a/Modules/AxB/AxB_BOM.xlsx
+++ b/Modules/AxB/AxB_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\AxB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75F306A-8ABC-4EB6-9A89-45ACA2CF04F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE388C4-0F75-4039-96CC-D38060DB9D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="132">
   <si>
     <t>Qty</t>
   </si>
@@ -131,39 +131,18 @@
     <t>Switching Diode</t>
   </si>
   <si>
-    <t>Parts in itallic are on the front PCB!</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
     <t>https://www.aliexpress.com/item/1005002670881002.html</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/cm-100n-x7r_100/mlcc-tht-capacitors/sr-passives/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/jrg-47u_35/tht-electrolytic-capacitors/jb-capacitors/jrg1v470m02500630115000b/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/1n4001-dio/tht-universal-diodes/diotec-semiconductor/1n4001/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/1n4148-dio/tht-universal-diodes/diotec-semiconductor/1n4148/</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/1005003256812123.html</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/tl074acn/tht-operational-amplifiers/texas-instruments/</t>
-  </si>
-  <si>
     <t>https://www.thonk.co.uk/shop/alpha-9mm-pots-dshaft/</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/l-937egw/tht-leds-3mm/kingbright-electronic/</t>
-  </si>
-  <si>
     <t>PJ398SM</t>
   </si>
   <si>
@@ -257,12 +236,6 @@
     <t>https://www.aliexpress.com/item/1005001557138121.html</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/zl202-80g/pin-headers/connfly/ds1021-2-40sf11/</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -293,9 +266,6 @@
     <t>47pF</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/cct-47p_50v/mlcc-tht-capacitors/sr-passives/ct40805n470j500f3r/</t>
-  </si>
-  <si>
     <t>C3, C4, C5, C6</t>
   </si>
   <si>
@@ -314,9 +284,6 @@
     <t>4-Quadrant Multiplier</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/ad633jrz/analog-multiplexers-and-switches/analog-devices/</t>
-  </si>
-  <si>
     <t>B50k</t>
   </si>
   <si>
@@ -335,15 +302,6 @@
     </r>
   </si>
   <si>
-    <t>P_ATN_A, P_ATN_B</t>
-  </si>
-  <si>
-    <t>LD_A, LD_B, LD_OUT</t>
-  </si>
-  <si>
-    <t>J_IN_A, J_IN_B, J_OUT</t>
-  </si>
-  <si>
     <t>1x4</t>
   </si>
   <si>
@@ -353,12 +311,6 @@
     <t>J_A3, J_A4</t>
   </si>
   <si>
-    <t>J_B1, J_B2</t>
-  </si>
-  <si>
-    <t>J_B3, J_B4</t>
-  </si>
-  <si>
     <t>SPDT ON-ON</t>
   </si>
   <si>
@@ -416,7 +368,303 @@
     <t>* Use the included extra nut as a washer between the switch and the panel.</t>
   </si>
   <si>
-    <t>SW_RCT_A, SW_RCT_B</t>
+    <r>
+      <t>Resistor Network THT,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4 Isolated Resistors</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/black-nuts-washers/</t>
+  </si>
+  <si>
+    <t>Thonkiconn</t>
+  </si>
+  <si>
+    <t>R-1/4W</t>
+  </si>
+  <si>
+    <t>Electrolytic Capacitor THT</t>
+  </si>
+  <si>
+    <t>E-P2.5mm 6.3x11.5mm</t>
+  </si>
+  <si>
+    <t>C-P5mm</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor THT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, R10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P_ATN_A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_ATN_B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LD_A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LD_B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LD_OUT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SW_RCT_A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SW_RCT_B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J_IN_A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_IN_B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_OUT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J_B1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>J_B3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J_B4</t>
+    </r>
   </si>
   <si>
     <r>
@@ -431,74 +679,110 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> R5, R6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R7, R8, R9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, R10</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Resistor Network THT,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 4 Isolated Resistors</t>
-    </r>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/black-nuts-washers/</t>
-  </si>
-  <si>
-    <t>Thonkiconn</t>
-  </si>
-  <si>
-    <t>R-1/4W</t>
-  </si>
-  <si>
-    <t>Electrolytic Capacitor THT</t>
-  </si>
-  <si>
-    <t>E-P2.5mm 6.3x11.5mm</t>
-  </si>
-  <si>
-    <t>C-P5mm</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor THT</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R6</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/cct-47p_50v/mlcc-tht-capacitors/sr-passives/ct40805n470j500f3r/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/cm-100n-x7r_100/mlcc-tht-capacitors/sr-passives/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/jrg-47u_35/tht-electrolytic-capacitors/jb-capacitors/jrg1v470m02500630115000b/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/1n4001-dio/tht-universal-diodes/diotec-semiconductor/1n4001/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/1n4148-dio/tht-universal-diodes/diotec-semiconductor/1n4148/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/tl074acn/tht-operational-amplifiers/texas-instruments/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/icvt-14p/standard-dip-sockets/connfly/ds1009-14at1nx-0a2/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/ad633jrz/analog-multiplexers-and-switches/analog-devices/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/l-937egw/tht-leds-3mm/kingbright-electronic/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/zl202-80g/pin-headers/connfly/ds1021-2-40sf11/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p046/73P0034/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p050/73P0038/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p052/73P0040/</t>
+  </si>
+  <si>
+    <t>https://www.buerklin.com/en/p/quadrios/wirewound-resistors/22p054/73P0042/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/zl262-3sg/pin-headers/connfly/ds1023-1-3s21/</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/zl262-4sg/pin-headers/connfly/ds1023-1-4s21/</t>
+  </si>
+  <si>
+    <t>Alt Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Parts  with underline are on the front PCB!</t>
+  </si>
+  <si>
+    <t>Avalon Harmonics AxB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,15 +928,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -681,6 +956,22 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1027,14 +1318,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1381,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E9"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,663 +1689,762 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="F12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>88</v>
       </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C19" t="s">
         <v>91</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
         <v>89</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="J19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="B20" t="s">
         <v>97</v>
       </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>102</v>
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>39</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
+        <v>39</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="E24" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="F24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+        <v>59</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>2</v>
       </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2</v>
-      </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>109</v>
+        <v>50</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F11" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F12" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F31" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F20" r:id="rId16" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
-    <hyperlink ref="F24" r:id="rId17" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
-    <hyperlink ref="P6" r:id="rId18" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
-    <hyperlink ref="P7" r:id="rId19" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
-    <hyperlink ref="F7" r:id="rId20" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
-    <hyperlink ref="F6" r:id="rId21" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
-    <hyperlink ref="F8" r:id="rId22" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
-    <hyperlink ref="F15" r:id="rId23" xr:uid="{850880ED-5B0D-4785-BD00-D263FDB1367B}"/>
-    <hyperlink ref="F16" r:id="rId24" xr:uid="{53562666-7339-4495-85C8-BCFF4A8BDBAF}"/>
-    <hyperlink ref="F21" r:id="rId25" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
-    <hyperlink ref="F23" r:id="rId26" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
-    <hyperlink ref="F18" r:id="rId27" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
-    <hyperlink ref="F2" r:id="rId28" xr:uid="{9E0ED9E0-C3A3-4348-BB6F-5C429B9E61E7}"/>
-    <hyperlink ref="F5" r:id="rId29" xr:uid="{AC848EF4-7FAB-4E48-AF09-F798B5BC950A}"/>
-    <hyperlink ref="F3" r:id="rId30" xr:uid="{238CA172-A99C-46CD-9FBB-BE7CBE8D9023}"/>
-    <hyperlink ref="F4" r:id="rId31" xr:uid="{7C381042-415D-491B-ACA4-70B1B604E6FF}"/>
-    <hyperlink ref="F32" r:id="rId32" xr:uid="{5285EE03-FF15-4800-B4FB-C302200D43C4}"/>
+    <hyperlink ref="F18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F29" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F31" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F32" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J23" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F21" r:id="rId10" xr:uid="{8471C66D-2803-4E39-A4C9-56382FB4FA7C}"/>
+    <hyperlink ref="F25" r:id="rId11" xr:uid="{6ABC6086-4872-4A5E-A074-AF133E043F03}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{0078F1D0-2252-4276-B4FA-F7758611CB55}"/>
+    <hyperlink ref="F8" r:id="rId13" xr:uid="{C63AEC0D-8CBC-4750-A708-A0BDA2E3A104}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{850880ED-5B0D-4785-BD00-D263FDB1367B}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{53562666-7339-4495-85C8-BCFF4A8BDBAF}"/>
+    <hyperlink ref="F22" r:id="rId16" xr:uid="{70623DF7-AD80-49BE-8BCF-99E43397C3C6}"/>
+    <hyperlink ref="J24" r:id="rId17" xr:uid="{10E960AF-C6C6-47C3-9E72-05533B5ED5AD}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{362C4AFE-495E-47D3-8980-A94395D8849C}"/>
+    <hyperlink ref="J3" r:id="rId19" xr:uid="{9E0ED9E0-C3A3-4348-BB6F-5C429B9E61E7}"/>
+    <hyperlink ref="J6" r:id="rId20" xr:uid="{AC848EF4-7FAB-4E48-AF09-F798B5BC950A}"/>
+    <hyperlink ref="J4" r:id="rId21" xr:uid="{238CA172-A99C-46CD-9FBB-BE7CBE8D9023}"/>
+    <hyperlink ref="J5" r:id="rId22" xr:uid="{7C381042-415D-491B-ACA4-70B1B604E6FF}"/>
+    <hyperlink ref="F33" r:id="rId23" xr:uid="{5285EE03-FF15-4800-B4FB-C302200D43C4}"/>
+    <hyperlink ref="J14" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F13" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F9" r:id="rId30" xr:uid="{1D4215ED-E169-427E-90FC-04FAE5A9B71D}"/>
+    <hyperlink ref="J7" r:id="rId31" xr:uid="{D56F3FC4-21F0-446F-A842-9A94AA04813F}"/>
+    <hyperlink ref="J8" r:id="rId32" xr:uid="{8C810300-BA98-4ED0-8B65-62815602E020}"/>
+    <hyperlink ref="F3" r:id="rId33" xr:uid="{977127FB-AC67-46C8-B0B1-0501C19A549A}"/>
+    <hyperlink ref="F4" r:id="rId34" xr:uid="{359AC861-5C21-4BF5-8FAD-ACC8E938C8D6}"/>
+    <hyperlink ref="F5" r:id="rId35" xr:uid="{3911DD1D-F5E3-40DF-975F-85923B0A46A2}"/>
+    <hyperlink ref="F6" r:id="rId36" xr:uid="{D2EB87A2-04E8-48FC-B49C-94AC093B082C}"/>
+    <hyperlink ref="F24" r:id="rId37" xr:uid="{5649177F-DDA8-4B6A-B3A4-79E4FAFB8310}"/>
+    <hyperlink ref="F23" r:id="rId38" xr:uid="{B5142C91-0B17-4672-B1DD-9DF602826583}"/>
+    <hyperlink ref="F14" r:id="rId39" xr:uid="{54A5E477-5B48-4EAE-A009-A3E26DFEBCB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update tab names in all BOMs, fix bi-color LED naming.
</commit_message>
<xml_diff>
--- a/Modules/AxB/AxB_BOM.xlsx
+++ b/Modules/AxB/AxB_BOM.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\AxB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE388C4-0F75-4039-96CC-D38060DB9D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3790C51B-51F4-4E0A-9D01-8820E3B6E0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AxB" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,9 +95,6 @@
     <t>LED Red/Green</t>
   </si>
   <si>
-    <t>LED 3mm Flat Bicolor</t>
-  </si>
-  <si>
     <t>L-937EGW</t>
   </si>
   <si>
@@ -776,6 +773,9 @@
   </si>
   <si>
     <t>Avalon Harmonics AxB</t>
+  </si>
+  <si>
+    <t>LED 3mm Dome Bicolor</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1676,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1691,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1711,11 +1711,11 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1726,19 +1726,19 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1746,22 +1746,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1769,22 +1769,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1795,19 +1795,19 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1815,22 +1815,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1841,19 +1841,19 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1861,22 +1861,22 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1887,19 +1887,19 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
         <v>101</v>
       </c>
-      <c r="D10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" t="s">
-        <v>102</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1910,19 +1910,19 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1933,19 +1933,19 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1956,19 +1956,19 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1976,22 +1976,22 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2002,19 +2002,19 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2022,22 +2022,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>82</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,22 +2045,22 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2068,22 +2068,22 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2091,22 +2091,22 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" t="s">
         <v>88</v>
       </c>
-      <c r="C19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="J19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2114,22 +2114,22 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2137,22 +2137,22 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
         <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>86</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2160,22 +2160,22 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2183,22 +2183,22 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2206,22 +2206,22 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2229,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -2241,10 +2241,10 @@
         <v>18</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2252,19 +2252,19 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
         <v>52</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>53</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="J27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2272,19 +2272,19 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>58</v>
       </c>
-      <c r="E28" t="s">
-        <v>59</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2292,19 +2292,19 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="J29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2312,19 +2312,19 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="J31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2332,19 +2332,19 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="J32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2352,19 +2352,19 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2372,34 +2372,34 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E34" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="J34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>